<commit_message>
Prior to sending out initial strategy to collaborators
</commit_message>
<xml_diff>
--- a/Initial_Search_Strategy_Query_Builder.xlsx
+++ b/Initial_Search_Strategy_Query_Builder.xlsx
@@ -84,7 +84,35 @@
     <t xml:space="preserve">Not currently</t>
   </si>
   <si>
-    <t xml:space="preserve">"suicid*[Title/Abstract]"</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">"suicid*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">[Title/Abstract]</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">No</t>
@@ -436,7 +464,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -474,6 +502,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -620,11 +654,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -632,24 +666,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -657,19 +687,19 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -677,6 +707,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -762,7 +796,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="B2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F1" activeCellId="5" sqref="F2:F4 F8:F11 F13:F15 F17:F20 F101:F102 F1"/>
+      <selection pane="bottomLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2689,7 +2723,7 @@
   <dimension ref="A1:S87"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="5" sqref="F2:F4 F8:F11 F13:F15 F17:F20 F101:F102 C4"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3057,7 +3091,7 @@
   <dimension ref="A1:C80"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="5" sqref="F2:F4 F8:F11 F13:F15 F17:F20 F101:F102 B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Update .~lock.Initial_Search_Strategy_Query_Builder.xlsx#, .~lock.PubMedSearchHistoryJan2023.csv#, and 10 more files...
</commit_message>
<xml_diff>
--- a/Initial_Search_Strategy_Query_Builder.xlsx
+++ b/Initial_Search_Strategy_Query_Builder.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="134">
   <si>
     <t xml:space="preserve">Domain</t>
   </si>
@@ -84,35 +84,7 @@
     <t xml:space="preserve">Not currently</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">"suicid*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">[Title/Abstract]</t>
-    </r>
+    <t xml:space="preserve">"suicid*"[Title/Abstract]</t>
   </si>
   <si>
     <t xml:space="preserve">No</t>
@@ -440,9 +412,6 @@
   </si>
   <si>
     <t xml:space="preserve">NOTES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=TEXTJOIN(" OR ",1,A1:A3)</t>
   </si>
   <si>
     <t xml:space="preserve">INCLUDE MeSH</t>
@@ -464,13 +433,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -493,19 +461,11 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FF70AD47"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -515,7 +475,6 @@
       <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -523,14 +482,12 @@
       <color rgb="FFFF8000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -538,7 +495,6 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -546,7 +502,6 @@
       <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -554,21 +509,18 @@
       <color rgb="FFED7D31"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -576,7 +528,6 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -621,7 +572,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -654,32 +605,32 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -687,19 +638,19 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -707,10 +658,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -793,10 +740,8 @@
   </sheetPr>
   <dimension ref="A1:G105"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="B2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -889,7 +834,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" s="2" customFormat="true" ht="23.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" s="2" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1120,7 +1065,7 @@
       <c r="D17" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="0" t="s">
         <v>35</v>
       </c>
       <c r="G17" s="3" t="s">
@@ -1192,10 +1137,10 @@
       <c r="C21" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="11"/>
+      <c r="E21" s="10"/>
       <c r="F21" s="2" t="s">
         <v>19</v>
       </c>
@@ -1210,10 +1155,10 @@
       <c r="C22" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D22" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E22" s="11"/>
+      <c r="E22" s="10"/>
       <c r="F22" s="2" t="s">
         <v>19</v>
       </c>
@@ -1228,10 +1173,10 @@
       <c r="C23" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D23" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="E23" s="11"/>
+      <c r="E23" s="10"/>
       <c r="F23" s="2" t="s">
         <v>19</v>
       </c>
@@ -1246,10 +1191,10 @@
       <c r="C24" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D24" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E24" s="11"/>
+      <c r="E24" s="10"/>
       <c r="F24" s="2" t="s">
         <v>19</v>
       </c>
@@ -1264,10 +1209,10 @@
       <c r="C25" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="D25" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E25" s="11"/>
+      <c r="E25" s="10"/>
       <c r="F25" s="2" t="s">
         <v>19</v>
       </c>
@@ -1282,10 +1227,10 @@
       <c r="C26" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="D26" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="E26" s="11"/>
+      <c r="E26" s="10"/>
       <c r="F26" s="2" t="s">
         <v>19</v>
       </c>
@@ -1300,10 +1245,10 @@
       <c r="C27" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="D27" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="E27" s="11"/>
+      <c r="E27" s="10"/>
       <c r="F27" s="2" t="s">
         <v>19</v>
       </c>
@@ -1318,10 +1263,10 @@
       <c r="C28" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D28" s="11" t="s">
+      <c r="D28" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="E28" s="11"/>
+      <c r="E28" s="10"/>
       <c r="F28" s="2" t="s">
         <v>19</v>
       </c>
@@ -1336,10 +1281,10 @@
       <c r="C29" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D29" s="11" t="s">
+      <c r="D29" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="E29" s="11"/>
+      <c r="E29" s="10"/>
       <c r="F29" s="2" t="s">
         <v>19</v>
       </c>
@@ -1354,10 +1299,10 @@
       <c r="C30" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D30" s="11" t="s">
+      <c r="D30" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E30" s="11"/>
+      <c r="E30" s="10"/>
       <c r="F30" s="2" t="s">
         <v>19</v>
       </c>
@@ -1372,10 +1317,10 @@
       <c r="C31" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D31" s="11" t="s">
+      <c r="D31" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="E31" s="11"/>
+      <c r="E31" s="10"/>
       <c r="F31" s="2" t="s">
         <v>19</v>
       </c>
@@ -1390,10 +1335,10 @@
       <c r="C32" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D32" s="11" t="s">
+      <c r="D32" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="E32" s="11"/>
+      <c r="E32" s="10"/>
       <c r="F32" s="2" t="s">
         <v>19</v>
       </c>
@@ -1408,10 +1353,10 @@
       <c r="C33" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D33" s="11" t="s">
+      <c r="D33" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="E33" s="11"/>
+      <c r="E33" s="10"/>
       <c r="F33" s="2" t="s">
         <v>19</v>
       </c>
@@ -1426,10 +1371,10 @@
       <c r="C34" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D34" s="11" t="s">
+      <c r="D34" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="E34" s="11"/>
+      <c r="E34" s="10"/>
       <c r="F34" s="2" t="s">
         <v>19</v>
       </c>
@@ -1444,10 +1389,10 @@
       <c r="C35" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D35" s="11" t="s">
+      <c r="D35" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="E35" s="11"/>
+      <c r="E35" s="10"/>
       <c r="F35" s="2" t="s">
         <v>19</v>
       </c>
@@ -1462,10 +1407,10 @@
       <c r="C36" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D36" s="11" t="s">
+      <c r="D36" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="E36" s="11"/>
+      <c r="E36" s="10"/>
       <c r="F36" s="2" t="s">
         <v>19</v>
       </c>
@@ -1480,10 +1425,10 @@
       <c r="C37" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D37" s="11" t="s">
+      <c r="D37" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="E37" s="11"/>
+      <c r="E37" s="10"/>
       <c r="F37" s="2" t="s">
         <v>19</v>
       </c>
@@ -1498,10 +1443,10 @@
       <c r="C38" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D38" s="11" t="s">
+      <c r="D38" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="E38" s="11"/>
+      <c r="E38" s="10"/>
       <c r="F38" s="2" t="s">
         <v>19</v>
       </c>
@@ -1516,10 +1461,10 @@
       <c r="C39" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D39" s="11" t="s">
+      <c r="D39" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="E39" s="11"/>
+      <c r="E39" s="10"/>
       <c r="F39" s="2" t="s">
         <v>19</v>
       </c>
@@ -1534,10 +1479,10 @@
       <c r="C40" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D40" s="11" t="s">
+      <c r="D40" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E40" s="11"/>
+      <c r="E40" s="10"/>
       <c r="F40" s="2" t="s">
         <v>19</v>
       </c>
@@ -1552,10 +1497,10 @@
       <c r="C41" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D41" s="11" t="s">
+      <c r="D41" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="E41" s="11"/>
+      <c r="E41" s="10"/>
       <c r="F41" s="2" t="s">
         <v>19</v>
       </c>
@@ -1570,10 +1515,10 @@
       <c r="C42" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D42" s="11" t="s">
+      <c r="D42" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="E42" s="11"/>
+      <c r="E42" s="10"/>
       <c r="F42" s="2" t="s">
         <v>19</v>
       </c>
@@ -1588,10 +1533,10 @@
       <c r="C43" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D43" s="11" t="s">
+      <c r="D43" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="E43" s="11"/>
+      <c r="E43" s="10"/>
       <c r="F43" s="2" t="s">
         <v>19</v>
       </c>
@@ -1606,10 +1551,10 @@
       <c r="C44" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D44" s="11" t="s">
+      <c r="D44" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="E44" s="11"/>
+      <c r="E44" s="10"/>
       <c r="F44" s="2" t="s">
         <v>19</v>
       </c>
@@ -1624,10 +1569,10 @@
       <c r="C45" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D45" s="11" t="s">
+      <c r="D45" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="E45" s="11"/>
+      <c r="E45" s="10"/>
       <c r="F45" s="2" t="s">
         <v>19</v>
       </c>
@@ -1642,10 +1587,10 @@
       <c r="C46" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D46" s="11" t="s">
+      <c r="D46" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E46" s="11"/>
+      <c r="E46" s="10"/>
       <c r="F46" s="2" t="s">
         <v>19</v>
       </c>
@@ -1660,10 +1605,10 @@
       <c r="C47" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D47" s="11" t="s">
+      <c r="D47" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="E47" s="11"/>
+      <c r="E47" s="10"/>
       <c r="F47" s="2" t="s">
         <v>19</v>
       </c>
@@ -1678,10 +1623,10 @@
       <c r="C48" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D48" s="11" t="s">
+      <c r="D48" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E48" s="11"/>
+      <c r="E48" s="10"/>
       <c r="F48" s="2" t="s">
         <v>19</v>
       </c>
@@ -1696,10 +1641,10 @@
       <c r="C49" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D49" s="11" t="s">
+      <c r="D49" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="E49" s="11"/>
+      <c r="E49" s="10"/>
       <c r="F49" s="2" t="s">
         <v>19</v>
       </c>
@@ -1714,10 +1659,10 @@
       <c r="C50" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D50" s="11" t="s">
+      <c r="D50" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="E50" s="11"/>
+      <c r="E50" s="10"/>
       <c r="F50" s="2" t="s">
         <v>19</v>
       </c>
@@ -1732,10 +1677,10 @@
       <c r="C51" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D51" s="11" t="s">
+      <c r="D51" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="E51" s="11"/>
+      <c r="E51" s="10"/>
       <c r="F51" s="2" t="s">
         <v>19</v>
       </c>
@@ -1750,10 +1695,10 @@
       <c r="C52" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D52" s="11" t="s">
+      <c r="D52" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E52" s="11"/>
+      <c r="E52" s="10"/>
       <c r="F52" s="2" t="s">
         <v>19</v>
       </c>
@@ -1768,10 +1713,10 @@
       <c r="C53" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D53" s="11" t="s">
+      <c r="D53" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="E53" s="11"/>
+      <c r="E53" s="10"/>
       <c r="F53" s="2" t="s">
         <v>19</v>
       </c>
@@ -1786,10 +1731,10 @@
       <c r="C54" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D54" s="11" t="s">
+      <c r="D54" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="E54" s="11"/>
+      <c r="E54" s="10"/>
       <c r="F54" s="2" t="s">
         <v>19</v>
       </c>
@@ -1804,10 +1749,10 @@
       <c r="C55" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D55" s="11" t="s">
+      <c r="D55" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="E55" s="11"/>
+      <c r="E55" s="10"/>
       <c r="F55" s="2" t="s">
         <v>19</v>
       </c>
@@ -1822,10 +1767,10 @@
       <c r="C56" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D56" s="11" t="s">
+      <c r="D56" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="E56" s="11"/>
+      <c r="E56" s="10"/>
       <c r="F56" s="2" t="s">
         <v>19</v>
       </c>
@@ -1840,10 +1785,10 @@
       <c r="C57" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D57" s="11" t="s">
+      <c r="D57" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="E57" s="11"/>
+      <c r="E57" s="10"/>
       <c r="F57" s="2" t="s">
         <v>19</v>
       </c>
@@ -1858,10 +1803,10 @@
       <c r="C58" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D58" s="11" t="s">
+      <c r="D58" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="E58" s="11"/>
+      <c r="E58" s="10"/>
       <c r="F58" s="2" t="s">
         <v>19</v>
       </c>
@@ -1876,10 +1821,10 @@
       <c r="C59" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D59" s="11" t="s">
+      <c r="D59" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="E59" s="11"/>
+      <c r="E59" s="10"/>
       <c r="F59" s="2" t="s">
         <v>19</v>
       </c>
@@ -1894,10 +1839,10 @@
       <c r="C60" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D60" s="11" t="s">
+      <c r="D60" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="E60" s="11"/>
+      <c r="E60" s="10"/>
       <c r="F60" s="2" t="s">
         <v>19</v>
       </c>
@@ -1912,10 +1857,10 @@
       <c r="C61" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D61" s="11" t="s">
+      <c r="D61" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="E61" s="11"/>
+      <c r="E61" s="10"/>
       <c r="F61" s="2" t="s">
         <v>19</v>
       </c>
@@ -1930,10 +1875,10 @@
       <c r="C62" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D62" s="11" t="s">
+      <c r="D62" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="E62" s="11"/>
+      <c r="E62" s="10"/>
       <c r="F62" s="2" t="s">
         <v>19</v>
       </c>
@@ -1948,10 +1893,10 @@
       <c r="C63" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D63" s="11" t="s">
+      <c r="D63" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="E63" s="11"/>
+      <c r="E63" s="10"/>
       <c r="F63" s="2" t="s">
         <v>19</v>
       </c>
@@ -1966,10 +1911,10 @@
       <c r="C64" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D64" s="11" t="s">
+      <c r="D64" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="E64" s="11"/>
+      <c r="E64" s="10"/>
       <c r="F64" s="2" t="s">
         <v>19</v>
       </c>
@@ -1984,10 +1929,10 @@
       <c r="C65" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D65" s="11" t="s">
+      <c r="D65" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="E65" s="11"/>
+      <c r="E65" s="10"/>
       <c r="F65" s="2" t="s">
         <v>19</v>
       </c>
@@ -2002,10 +1947,10 @@
       <c r="C66" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D66" s="11" t="s">
+      <c r="D66" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="E66" s="11"/>
+      <c r="E66" s="10"/>
       <c r="F66" s="2" t="s">
         <v>19</v>
       </c>
@@ -2020,10 +1965,10 @@
       <c r="C67" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D67" s="11" t="s">
+      <c r="D67" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="E67" s="11"/>
+      <c r="E67" s="10"/>
       <c r="F67" s="2" t="s">
         <v>19</v>
       </c>
@@ -2038,10 +1983,10 @@
       <c r="C68" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D68" s="11" t="s">
+      <c r="D68" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="E68" s="11"/>
+      <c r="E68" s="10"/>
       <c r="F68" s="2" t="s">
         <v>19</v>
       </c>
@@ -2056,10 +2001,10 @@
       <c r="C69" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D69" s="11" t="s">
+      <c r="D69" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="E69" s="11"/>
+      <c r="E69" s="10"/>
       <c r="F69" s="2" t="s">
         <v>19</v>
       </c>
@@ -2074,10 +2019,10 @@
       <c r="C70" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D70" s="11" t="s">
+      <c r="D70" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="E70" s="11"/>
+      <c r="E70" s="10"/>
       <c r="F70" s="2" t="s">
         <v>19</v>
       </c>
@@ -2109,10 +2054,10 @@
       <c r="C72" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D72" s="11" t="s">
+      <c r="D72" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="E72" s="11"/>
+      <c r="E72" s="10"/>
       <c r="F72" s="2" t="s">
         <v>19</v>
       </c>
@@ -2127,10 +2072,10 @@
       <c r="C73" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D73" s="11" t="s">
+      <c r="D73" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="E73" s="11"/>
+      <c r="E73" s="10"/>
       <c r="F73" s="2" t="s">
         <v>19</v>
       </c>
@@ -2145,10 +2090,10 @@
       <c r="C74" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D74" s="11" t="s">
+      <c r="D74" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="E74" s="11"/>
+      <c r="E74" s="10"/>
       <c r="F74" s="2" t="s">
         <v>19</v>
       </c>
@@ -2163,10 +2108,10 @@
       <c r="C75" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D75" s="11" t="s">
+      <c r="D75" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="E75" s="11"/>
+      <c r="E75" s="10"/>
       <c r="F75" s="2" t="s">
         <v>19</v>
       </c>
@@ -2181,10 +2126,10 @@
       <c r="C76" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D76" s="11" t="s">
+      <c r="D76" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="E76" s="11"/>
+      <c r="E76" s="10"/>
       <c r="F76" s="2" t="s">
         <v>19</v>
       </c>
@@ -2199,10 +2144,10 @@
       <c r="C77" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D77" s="11" t="s">
+      <c r="D77" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="E77" s="11"/>
+      <c r="E77" s="10"/>
       <c r="F77" s="2" t="s">
         <v>19</v>
       </c>
@@ -2217,10 +2162,10 @@
       <c r="C78" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D78" s="11" t="s">
+      <c r="D78" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="E78" s="11"/>
+      <c r="E78" s="10"/>
       <c r="F78" s="2" t="s">
         <v>19</v>
       </c>
@@ -2235,10 +2180,10 @@
       <c r="C79" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D79" s="11" t="s">
+      <c r="D79" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="E79" s="11"/>
+      <c r="E79" s="10"/>
       <c r="F79" s="2" t="s">
         <v>19</v>
       </c>
@@ -2253,10 +2198,10 @@
       <c r="C80" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D80" s="11" t="s">
+      <c r="D80" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="E80" s="11"/>
+      <c r="E80" s="10"/>
       <c r="F80" s="2" t="s">
         <v>19</v>
       </c>
@@ -2271,10 +2216,10 @@
       <c r="C81" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D81" s="11" t="s">
+      <c r="D81" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="E81" s="11"/>
+      <c r="E81" s="10"/>
       <c r="F81" s="2" t="s">
         <v>19</v>
       </c>
@@ -2289,10 +2234,10 @@
       <c r="C82" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D82" s="11" t="s">
+      <c r="D82" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="E82" s="11"/>
+      <c r="E82" s="10"/>
       <c r="F82" s="2" t="s">
         <v>19</v>
       </c>
@@ -2307,10 +2252,10 @@
       <c r="C83" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D83" s="11" t="s">
+      <c r="D83" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="E83" s="11"/>
+      <c r="E83" s="10"/>
       <c r="F83" s="2" t="s">
         <v>19</v>
       </c>
@@ -2325,10 +2270,10 @@
       <c r="C84" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D84" s="11" t="s">
+      <c r="D84" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="E84" s="11"/>
+      <c r="E84" s="10"/>
       <c r="F84" s="2" t="s">
         <v>19</v>
       </c>
@@ -2343,10 +2288,10 @@
       <c r="C85" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D85" s="11" t="s">
+      <c r="D85" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="E85" s="11"/>
+      <c r="E85" s="10"/>
       <c r="F85" s="2" t="s">
         <v>19</v>
       </c>
@@ -2361,10 +2306,10 @@
       <c r="C86" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D86" s="11" t="s">
+      <c r="D86" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="E86" s="11"/>
+      <c r="E86" s="10"/>
       <c r="F86" s="2" t="s">
         <v>19</v>
       </c>
@@ -2379,10 +2324,10 @@
       <c r="C87" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D87" s="11" t="s">
+      <c r="D87" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="E87" s="11"/>
+      <c r="E87" s="10"/>
       <c r="F87" s="2" t="s">
         <v>19</v>
       </c>
@@ -2397,10 +2342,10 @@
       <c r="C88" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D88" s="11" t="s">
+      <c r="D88" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="E88" s="11"/>
+      <c r="E88" s="10"/>
       <c r="F88" s="2" t="s">
         <v>19</v>
       </c>
@@ -2415,10 +2360,10 @@
       <c r="C89" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D89" s="11" t="s">
+      <c r="D89" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="E89" s="11"/>
+      <c r="E89" s="10"/>
       <c r="F89" s="2" t="s">
         <v>19</v>
       </c>
@@ -2433,10 +2378,10 @@
       <c r="C90" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D90" s="11" t="s">
+      <c r="D90" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="E90" s="11"/>
+      <c r="E90" s="10"/>
       <c r="F90" s="2" t="s">
         <v>19</v>
       </c>
@@ -2451,10 +2396,10 @@
       <c r="C91" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D91" s="11" t="s">
+      <c r="D91" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="E91" s="11"/>
+      <c r="E91" s="10"/>
       <c r="F91" s="2" t="s">
         <v>19</v>
       </c>
@@ -2469,10 +2414,10 @@
       <c r="C92" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D92" s="11" t="s">
+      <c r="D92" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="E92" s="11"/>
+      <c r="E92" s="10"/>
       <c r="F92" s="2" t="s">
         <v>19</v>
       </c>
@@ -2487,10 +2432,10 @@
       <c r="C93" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D93" s="11" t="s">
+      <c r="D93" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="E93" s="11"/>
+      <c r="E93" s="10"/>
       <c r="F93" s="2" t="s">
         <v>19</v>
       </c>
@@ -2505,10 +2450,10 @@
       <c r="C94" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D94" s="11" t="s">
+      <c r="D94" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="E94" s="11"/>
+      <c r="E94" s="10"/>
       <c r="F94" s="2" t="s">
         <v>19</v>
       </c>
@@ -2523,10 +2468,10 @@
       <c r="C95" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D95" s="11" t="s">
+      <c r="D95" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="E95" s="11"/>
+      <c r="E95" s="10"/>
       <c r="F95" s="2" t="s">
         <v>19</v>
       </c>
@@ -2541,10 +2486,10 @@
       <c r="C96" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D96" s="11" t="s">
+      <c r="D96" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="E96" s="11"/>
+      <c r="E96" s="10"/>
       <c r="F96" s="2" t="s">
         <v>19</v>
       </c>
@@ -2559,10 +2504,10 @@
       <c r="C97" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D97" s="11" t="s">
+      <c r="D97" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="E97" s="11"/>
+      <c r="E97" s="10"/>
       <c r="F97" s="2" t="s">
         <v>19</v>
       </c>
@@ -2577,10 +2522,10 @@
       <c r="C98" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D98" s="11" t="s">
+      <c r="D98" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="E98" s="11"/>
+      <c r="E98" s="10"/>
       <c r="F98" s="2" t="s">
         <v>19</v>
       </c>
@@ -2595,10 +2540,10 @@
       <c r="C99" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D99" s="11" t="s">
+      <c r="D99" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="E99" s="11"/>
+      <c r="E99" s="10"/>
       <c r="F99" s="2" t="s">
         <v>19</v>
       </c>
@@ -2613,10 +2558,10 @@
       <c r="C100" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D100" s="11" t="s">
+      <c r="D100" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="E100" s="11"/>
+      <c r="E100" s="10"/>
       <c r="F100" s="2" t="s">
         <v>19</v>
       </c>
@@ -2625,13 +2570,13 @@
       <c r="A101" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B101" s="12" t="s">
+      <c r="B101" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C101" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D101" s="11" t="s">
+      <c r="C101" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D101" s="10" t="s">
         <v>121</v>
       </c>
       <c r="F101" s="2" t="s">
@@ -2642,13 +2587,13 @@
       <c r="A102" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B102" s="12" t="s">
+      <c r="B102" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C102" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D102" s="11" t="s">
+      <c r="C102" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D102" s="10" t="s">
         <v>123</v>
       </c>
       <c r="F102" s="2" t="s">
@@ -2659,13 +2604,13 @@
       <c r="A103" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B103" s="14" t="s">
+      <c r="B103" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C103" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D103" s="11" t="s">
+      <c r="C103" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D103" s="10" t="s">
         <v>124</v>
       </c>
       <c r="F103" s="0"/>
@@ -2674,13 +2619,13 @@
       <c r="A104" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B104" s="14" t="s">
+      <c r="B104" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C104" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D104" s="11" t="s">
+      <c r="C104" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D104" s="10" t="s">
         <v>125</v>
       </c>
       <c r="F104" s="2" t="s">
@@ -2691,13 +2636,13 @@
       <c r="A105" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B105" s="14" t="s">
+      <c r="B105" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C105" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D105" s="11" t="s">
+      <c r="C105" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D105" s="10" t="s">
         <v>126</v>
       </c>
       <c r="F105" s="2" t="s">
@@ -2722,21 +2667,20 @@
   </sheetPr>
   <dimension ref="A1:S87"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="36.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="41.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="37.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="29.86"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="65" style="10" width="8.67"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="1" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
         <v>127</v>
       </c>
@@ -2749,14 +2693,15 @@
       <c r="D1" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="5" t="str">
+        <f aca="false">_xlfn.TEXTJOIN(" OR ",1,A1:A3)</f>
+        <v>Inclusion/Exclusion OR INCLUDE MeSH OR INCLUDE MeSH</v>
+      </c>
+      <c r="F1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="15" t="s">
         <v>130</v>
-      </c>
-      <c r="F1" s="0"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="16" t="s">
-        <v>131</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>39</v>
@@ -2764,11 +2709,11 @@
       <c r="C2" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="11"/>
+      <c r="D2" s="10"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="16" t="s">
-        <v>131</v>
+      <c r="A3" s="15" t="s">
+        <v>130</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>40</v>
@@ -2776,301 +2721,301 @@
       <c r="C3" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="11"/>
+      <c r="D3" s="10"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="16" t="s">
-        <v>131</v>
+      <c r="A4" s="15" t="s">
+        <v>130</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>37</v>
       </c>
       <c r="C4" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="D4" s="10"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="16" t="s">
         <v>132</v>
-      </c>
-      <c r="D4" s="11"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="17" t="s">
-        <v>133</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="D5" s="11"/>
+      <c r="C5" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D5" s="10"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="19"/>
-      <c r="D6" s="11"/>
+      <c r="A6" s="18"/>
+      <c r="D6" s="10"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D7" s="11"/>
+      <c r="D7" s="10"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D8" s="11"/>
+      <c r="D8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D9" s="11"/>
+      <c r="D9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D10" s="11"/>
+      <c r="D10" s="10"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="11"/>
+      <c r="D11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D12" s="11"/>
+      <c r="D12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D13" s="11"/>
+      <c r="D13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D14" s="11"/>
+      <c r="D14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D15" s="11"/>
+      <c r="D15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D16" s="20"/>
+      <c r="D16" s="19"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D17" s="21"/>
+      <c r="D17" s="20"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D18" s="20"/>
+      <c r="D18" s="19"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D19" s="20"/>
+      <c r="D19" s="19"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D20" s="20"/>
+      <c r="D20" s="19"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D21" s="20"/>
+      <c r="D21" s="19"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D22" s="11"/>
+      <c r="D22" s="10"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D23" s="11"/>
+      <c r="D23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D24" s="11"/>
+      <c r="D24" s="10"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D25" s="11"/>
+      <c r="D25" s="10"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C26" s="20"/>
-      <c r="D26" s="11"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="10"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="21"/>
-      <c r="D27" s="11"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="10"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="20"/>
-      <c r="D28" s="11"/>
-      <c r="S28" s="22" t="n">
+      <c r="C28" s="19"/>
+      <c r="D28" s="10"/>
+      <c r="S28" s="21" t="n">
         <v>24</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="20"/>
-      <c r="D29" s="11"/>
-      <c r="S29" s="22" t="n">
+      <c r="C29" s="19"/>
+      <c r="D29" s="10"/>
+      <c r="S29" s="21" t="n">
         <v>293</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="20"/>
-      <c r="D30" s="11"/>
-      <c r="S30" s="22" t="n">
+      <c r="C30" s="19"/>
+      <c r="D30" s="10"/>
+      <c r="S30" s="21" t="n">
         <v>1349</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D31" s="11"/>
-      <c r="S31" s="22" t="n">
+      <c r="D31" s="10"/>
+      <c r="S31" s="21" t="n">
         <v>343</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D32" s="11"/>
-      <c r="S32" s="22" t="n">
+      <c r="D32" s="10"/>
+      <c r="S32" s="21" t="n">
         <v>349</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D33" s="11"/>
+      <c r="D33" s="10"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D34" s="11"/>
+      <c r="D34" s="10"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D35" s="11"/>
+      <c r="D35" s="10"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D36" s="11"/>
+      <c r="D36" s="10"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D37" s="11"/>
+      <c r="D37" s="10"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D38" s="11"/>
+      <c r="D38" s="10"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D39" s="11"/>
+      <c r="D39" s="10"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D40" s="11"/>
+      <c r="D40" s="10"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D41" s="11"/>
+      <c r="D41" s="10"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D42" s="11"/>
+      <c r="D42" s="10"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D43" s="11"/>
+      <c r="D43" s="10"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D44" s="11"/>
+      <c r="D44" s="10"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D45" s="11"/>
+      <c r="D45" s="10"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D46" s="11"/>
+      <c r="D46" s="10"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D47" s="11"/>
+      <c r="D47" s="10"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D48" s="11"/>
+      <c r="D48" s="10"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D49" s="11"/>
+      <c r="D49" s="10"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D50" s="11"/>
+      <c r="D50" s="10"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D51" s="11"/>
+      <c r="D51" s="10"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D52" s="11"/>
+      <c r="D52" s="10"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D53" s="11"/>
+      <c r="D53" s="10"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D54" s="11"/>
+      <c r="D54" s="10"/>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D55" s="11"/>
+      <c r="D55" s="10"/>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D56" s="11"/>
+      <c r="D56" s="10"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D57" s="11"/>
+      <c r="D57" s="10"/>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D58" s="11"/>
+      <c r="D58" s="10"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D59" s="11"/>
+      <c r="D59" s="10"/>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D60" s="11"/>
+      <c r="D60" s="10"/>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D61" s="11"/>
+      <c r="D61" s="10"/>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D62" s="11"/>
+      <c r="D62" s="10"/>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D63" s="11"/>
+      <c r="D63" s="10"/>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D64" s="11"/>
+      <c r="D64" s="10"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D65" s="11"/>
+      <c r="D65" s="10"/>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D66" s="11"/>
+      <c r="D66" s="10"/>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D67" s="11"/>
+      <c r="D67" s="10"/>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D68" s="11"/>
+      <c r="D68" s="10"/>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D69" s="11"/>
+      <c r="D69" s="10"/>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D70" s="11"/>
+      <c r="D70" s="10"/>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D71" s="11"/>
+      <c r="D71" s="10"/>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D72" s="11"/>
+      <c r="D72" s="10"/>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D73" s="11"/>
+      <c r="D73" s="10"/>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D74" s="11"/>
+      <c r="D74" s="10"/>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D75" s="11"/>
+      <c r="D75" s="10"/>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D76" s="11"/>
+      <c r="D76" s="10"/>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D77" s="11"/>
+      <c r="D77" s="10"/>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D78" s="11"/>
+      <c r="D78" s="10"/>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D79" s="11"/>
+      <c r="D79" s="10"/>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D80" s="11"/>
+      <c r="D80" s="10"/>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D81" s="11"/>
+      <c r="D81" s="10"/>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D82" s="11"/>
+      <c r="D82" s="10"/>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D83" s="11"/>
+      <c r="D83" s="10"/>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D84" s="11"/>
+      <c r="D84" s="10"/>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D85" s="11"/>
-    </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D86" s="11"/>
-    </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D87" s="11"/>
+      <c r="D85" s="10"/>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D86" s="10"/>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D87" s="10"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3090,429 +3035,428 @@
   </sheetPr>
   <dimension ref="A1:C80"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="52.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="39.7"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="65" style="10" width="8.67"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="11" t="s">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="11" t="s">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="11" t="s">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="10" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="11" t="s">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="10" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="11" t="s">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="10" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="11" t="s">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="10" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="11" t="s">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="10" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11" t="s">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="10" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11" t="s">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="10" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="11" t="s">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="10" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="11" t="s">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="10" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="11" t="s">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="11" t="s">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="10" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="11" t="s">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="10" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="11" t="s">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="10" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="11" t="s">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="10" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="11" t="s">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="10" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="11" t="s">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="10" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="11" t="s">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="10" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="11" t="s">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="10" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="11" t="s">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="10" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="11" t="s">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="10" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="11" t="s">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="10" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="11" t="s">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="11" t="s">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="10" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="11" t="s">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="10" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="11" t="s">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="10" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="11" t="s">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="10" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="11" t="s">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="10" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="11" t="s">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="10" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="11" t="s">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="10" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="11" t="s">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="10" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="11" t="s">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="10" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="11" t="s">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="10" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="11" t="s">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="10" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="11" t="s">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="10" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="11" t="s">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="10" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="11" t="s">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="10" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="11" t="s">
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="10" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="11" t="s">
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="10" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="11" t="s">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="10" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="11" t="s">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="10" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="11" t="s">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="10" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="11" t="s">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="10" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="11" t="s">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="10" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="11" t="s">
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="10" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="11" t="s">
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="10" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="11" t="s">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="10" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="11" t="s">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="10" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="11" t="s">
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="10" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="11" t="s">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="10" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="11" t="s">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="10" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="11" t="s">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="10" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="11" t="s">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="10" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="11" t="s">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="10" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="11" t="s">
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="10" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="11" t="s">
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="10" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="11" t="s">
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="10" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="11" t="s">
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="10" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="11" t="s">
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="10" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="11" t="s">
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="10" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="11" t="s">
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="10" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="11" t="s">
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="10" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="11" t="s">
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="10" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="11" t="s">
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="10" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="11" t="s">
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="10" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="11" t="s">
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="10" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="11" t="s">
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="10" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="11" t="s">
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="10" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="11" t="s">
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="10" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="11" t="s">
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="10" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="11" t="s">
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="10" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="11" t="s">
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="10" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="11" t="s">
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="11" t="s">
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="10" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="11" t="s">
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="10" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="11" t="s">
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="10" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="11" t="s">
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="10" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
         <v>91</v>
       </c>

</xml_diff>